<commit_message>
instruct how to add vacancy
</commit_message>
<xml_diff>
--- a/OrangeHRM/bin/Debug/TestCaseData.xlsx
+++ b/OrangeHRM/bin/Debug/TestCaseData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuongmt\OneDrive\Tài liệu\Huflit\SQualityAssurance\LT\Selenium\OrangeHRM\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3115B627-4BE9-42D0-83CC-C664A8962DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A748F69F-EEB6-4C11-B9F7-B0B679967BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidUser" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>username</t>
   </si>
@@ -66,10 +66,7 @@
     <t>hiringManager</t>
   </si>
   <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Web developer</t>
+    <t>Test3</t>
   </si>
   <si>
     <t xml:space="preserve">Tuong  Ma</t>
@@ -394,7 +391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -534,14 +531,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA3E80F-7DE0-4317-9875-6CC0AD481508}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" bestFit="1" width="9" customWidth="1"/>
     <col min="2" max="2" bestFit="1" width="10" customWidth="1"/>
     <col min="3" max="3" bestFit="1" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" bestFit="1" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -578,10 +578,10 @@
         <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add check condition and write fail condition to excel
</commit_message>
<xml_diff>
--- a/OrangeHRM/bin/Debug/TestCaseData.xlsx
+++ b/OrangeHRM/bin/Debug/TestCaseData.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuongmt\OneDrive\Tài liệu\Huflit\SQualityAssurance\LT\Selenium\OrangeHRM\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090E3ACC-F2C1-4892-8273-A413F386F3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2F9CEB-67E9-491C-A74F-E40D84B89157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidUser" sheetId="1" r:id="rId1"/>
     <sheet name="InvalidUser" sheetId="2" r:id="rId2"/>
     <sheet name="AddJobTitle" sheetId="4" r:id="rId3"/>
     <sheet name="AddVacancy" sheetId="3" r:id="rId4"/>
-    <sheet name="AddCandidate" sheetId="5" r:id="rId5"/>
+    <sheet name="DeleteVacancy" sheetId="7" r:id="rId5"/>
+    <sheet name="AddCandidate" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="43">
   <si>
     <t>username</t>
   </si>
@@ -52,25 +53,73 @@
     <t>Pass</t>
   </si>
   <si>
+    <t>Tuong*124</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Fail (Invalid credentials)</t>
+  </si>
+  <si>
     <t>tuong</t>
   </si>
   <si>
     <t>jobTitle</t>
   </si>
   <si>
+    <t>Database developer</t>
+  </si>
+  <si>
+    <t>Database developer1</t>
+  </si>
+  <si>
+    <t>Fail (Job Title is exist)</t>
+  </si>
+  <si>
+    <t>vacancyName</t>
+  </si>
+  <si>
+    <t>hiringManager</t>
+  </si>
+  <si>
+    <t>Tester5</t>
+  </si>
+  <si>
     <t>Software developer</t>
   </si>
   <si>
-    <t>vacancyName</t>
-  </si>
-  <si>
-    <t>hiringManager</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tuong  Ma</t>
+    <t>Tuong  Ma</t>
+  </si>
+  <si>
+    <t>Tester0109</t>
+  </si>
+  <si>
+    <t>Fail (Vacancy Name is exist)</t>
+  </si>
+  <si>
+    <t>Tester6</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Fail (Job Title isn't exist)</t>
+  </si>
+  <si>
+    <t>Tester7</t>
+  </si>
+  <si>
+    <t>Tan Duong</t>
+  </si>
+  <si>
+    <t>Fail (Hiring Manager isn't exist)</t>
+  </si>
+  <si>
+    <t>vacancyNo</t>
+  </si>
+  <si>
+    <t>Fail (Vacancy No not found)</t>
   </si>
   <si>
     <t>firstName</t>
@@ -101,14 +150,22 @@
   </si>
   <si>
     <t>tuantuong326@gmail.com</t>
+  </si>
+  <si>
+    <t>Fail (Vacancy not found)</t>
+  </si>
+  <si>
+    <t>tuantuong326@gmai</t>
+  </si>
+  <si>
+    <t>Fail (Email is invalid format)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,17 +188,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF1F1F1F"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF1F1F1F"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,15 +224,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" applyNumberFormat="0" fontId="2" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -453,225 +517,412 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0538FAA-1A95-4A67-9E65-9049219346AD}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="0">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
         <v>123456</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F1CF16-D497-4199-9696-F19E7C9263E8}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="9" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="10" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>9</v>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA3E80F-7DE0-4317-9875-6CC0AD481508}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="9" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="10" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" bestFit="1" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" bestFit="1" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="0" t="s">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>13</v>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4AD822-807E-493C-9A4A-D49C23BDC73E}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F03B891-B879-4A0A-BEF2-CA155E95A337}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="1" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="9.33203125" customWidth="1"/>
-    <col min="4" max="5" width="9.33203125" customWidth="1"/>
-    <col min="6" max="6" bestFit="1" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" bestFit="1" width="22.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="7">
+        <v>333</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4AD822-807E-493C-9A4A-D49C23BDC73E}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -679,19 +930,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>2</v>
@@ -700,7 +951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -708,28 +959,84 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="G3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
done delete candidate, set suitable window (change window size to test responsive, some page will change class and component when change window size)
</commit_message>
<xml_diff>
--- a/OrangeHRM/bin/Debug/TestCaseData.xlsx
+++ b/OrangeHRM/bin/Debug/TestCaseData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuongmt\OneDrive\Tài liệu\Huflit\SQualityAssurance\LT\Selenium\OrangeHRM\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2F9CEB-67E9-491C-A74F-E40D84B89157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFF3049-8AD3-4069-AA48-69F15AEB0BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidUser" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="AddVacancy" sheetId="3" r:id="rId4"/>
     <sheet name="DeleteVacancy" sheetId="7" r:id="rId5"/>
     <sheet name="AddCandidate" sheetId="5" r:id="rId6"/>
+    <sheet name="DeleteCandidate" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>username</t>
   </si>
@@ -89,7 +90,7 @@
     <t>Software developer</t>
   </si>
   <si>
-    <t>Tuong  Ma</t>
+    <t xml:space="preserve">Tuong  Ma</t>
   </si>
   <si>
     <t>Tester0109</t>
@@ -159,13 +160,20 @@
   </si>
   <si>
     <t>Fail (Email is invalid format)</t>
+  </si>
+  <si>
+    <t>candidateNo</t>
+  </si>
+  <si>
+    <t>Fail (Candidate No not found)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,18 +232,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="2" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -525,54 +533,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="10" customWidth="1"/>
+    <col min="4" max="4" bestFit="1" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -586,47 +595,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>123456</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -640,73 +650,74 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="9" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="10" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="22" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -720,119 +731,120 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="9" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="10" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" bestFit="1" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="0" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="0" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -841,51 +853,51 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="9" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="10" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" bestFit="1" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" bestFit="1" width="6.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -895,12 +907,13 @@
       <c r="C3" s="7">
         <v>333</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -908,21 +921,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4AD822-807E-493C-9A4A-D49C23BDC73E}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="9.33203125" customWidth="1"/>
     <col min="4" max="5" width="9.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" bestFit="1" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" bestFit="1" width="22.88671875" customWidth="1" style="6"/>
+    <col min="8" max="8" bestFit="1" width="6.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -951,7 +964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -978,7 +991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1000,11 +1013,11 @@
       <c r="G3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1026,17 +1039,82 @@
       <c r="G4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="0" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81815B1-E3AD-453F-AFA8-92B78834875B}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" bestFit="1" width="11.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>333</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>